<commit_message>
Fixing_ the big mistake
</commit_message>
<xml_diff>
--- a/Data_science_outputs/1000pop/Monthly_consumption/Montlhy_consumption_2.xlsx
+++ b/Data_science_outputs/1000pop/Monthly_consumption/Montlhy_consumption_2.xlsx
@@ -475,13 +475,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>13002.02504835002</v>
+        <v>7873.70901350002</v>
       </c>
       <c r="C2" t="n">
         <v>1284.160040933338</v>
       </c>
       <c r="D2" t="n">
-        <v>5620.1298545</v>
+        <v>505.2825002833334</v>
       </c>
       <c r="E2" t="n">
         <v>1676.905915283333</v>
@@ -498,13 +498,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>12178.82287296668</v>
+        <v>7366.369618183351</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>5267.600863866667</v>
+        <v>479.8452055333333</v>
       </c>
       <c r="E3" t="n">
         <v>1578.406598766667</v>
@@ -521,13 +521,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>13013.99136781669</v>
+        <v>7900.730378083354</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>5616.20888295</v>
+        <v>529.6545940666667</v>
       </c>
       <c r="E4" t="n">
         <v>1660.9716132</v>
@@ -544,13 +544,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>12587.46695600002</v>
+        <v>7617.880432633352</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>5462.40290425</v>
+        <v>495.8968661333333</v>
       </c>
       <c r="E5" t="n">
         <v>1642.590426733333</v>
@@ -567,13 +567,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>13004.17868440002</v>
+        <v>7903.597525466686</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>5624.559847699999</v>
+        <v>523.54358935</v>
       </c>
       <c r="E6" t="n">
         <v>1691.5564533</v>
@@ -590,13 +590,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>12620.42237966669</v>
+        <v>7655.652308883353</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>5452.220863683333</v>
+        <v>509.1682569166667</v>
       </c>
       <c r="E7" t="n">
         <v>1642.30097235</v>
@@ -613,13 +613,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>12989.57492838335</v>
+        <v>7895.98543095002</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>5634.44593295</v>
+        <v>518.8358951499999</v>
       </c>
       <c r="E8" t="n">
         <v>1685.754952883333</v>
@@ -636,13 +636,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>13031.12298213335</v>
+        <v>7895.23621675002</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>5640.491981516666</v>
+        <v>523.1529089666667</v>
       </c>
       <c r="E9" t="n">
         <v>1674.454914216667</v>
@@ -659,13 +659,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>12587.78195543335</v>
+        <v>7664.542564450019</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>5444.632163233334</v>
+        <v>500.90419505</v>
       </c>
       <c r="E10" t="n">
         <v>1623.315652</v>
@@ -682,13 +682,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>12988.62234153335</v>
+        <v>7893.204864216686</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>5630.200543733334</v>
+        <v>523.8685568833333</v>
       </c>
       <c r="E11" t="n">
         <v>1675.234227316667</v>
@@ -705,13 +705,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>12557.58448108335</v>
+        <v>7666.541936400019</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>5466.12425375</v>
+        <v>492.1805045666667</v>
       </c>
       <c r="E12" t="n">
         <v>1634.68876465</v>
@@ -728,13 +728,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>12588.80800785002</v>
+        <v>7641.802333766685</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>5434.568201499999</v>
+        <v>504.9592266333333</v>
       </c>
       <c r="E13" t="n">
         <v>1643.7542065</v>

</xml_diff>